<commit_message>
Final Check for Config
</commit_message>
<xml_diff>
--- a/rsc/Mapping.xlsx
+++ b/rsc/Mapping.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\مشروع التخرج\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Final Project\Solution\MedicalSystem\rsc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D0EE273-6190-44C1-8D7A-2F8B41911676}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6335310-4135-423E-9A36-36C385A01A39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{713BCA83-253F-4A29-8423-38F84BDA3CEA}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="65">
   <si>
     <t>Hospital</t>
   </si>
@@ -225,6 +225,12 @@
   </si>
   <si>
     <t>EntityType</t>
+  </si>
+  <si>
+    <t>MedTypeID</t>
+  </si>
+  <si>
+    <t>ShiftID</t>
   </si>
 </sst>
 </file>
@@ -402,6 +408,12 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -418,12 +430,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -742,8 +748,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{080D48B2-ECE1-4924-B2B9-306A26AF896E}">
   <dimension ref="D4:L59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="Q16" sqref="Q16"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -840,7 +846,7 @@
       <c r="I13" s="10"/>
       <c r="J13" s="10"/>
       <c r="K13" s="10"/>
-      <c r="L13" s="18"/>
+      <c r="L13" s="12"/>
     </row>
     <row r="14" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D14" s="1" t="s">
@@ -872,12 +878,12 @@
       </c>
     </row>
     <row r="16" spans="4:12" x14ac:dyDescent="0.3">
-      <c r="D16" s="17" t="s">
+      <c r="D16" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E16" s="17"/>
-      <c r="F16" s="17"/>
-      <c r="G16" s="17"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
     </row>
     <row r="17" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D17" s="2" t="s">
@@ -894,13 +900,13 @@
       </c>
     </row>
     <row r="19" spans="4:12" x14ac:dyDescent="0.3">
-      <c r="D19" s="15" t="s">
+      <c r="D19" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="E19" s="15"/>
-      <c r="F19" s="15"/>
-      <c r="G19" s="15"/>
-      <c r="H19" s="15"/>
+      <c r="E19" s="17"/>
+      <c r="F19" s="17"/>
+      <c r="G19" s="17"/>
+      <c r="H19" s="17"/>
     </row>
     <row r="20" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D20" s="3" t="s">
@@ -920,10 +926,10 @@
       </c>
     </row>
     <row r="22" spans="4:12" x14ac:dyDescent="0.3">
-      <c r="D22" s="15" t="s">
+      <c r="D22" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="E22" s="15"/>
+      <c r="E22" s="17"/>
     </row>
     <row r="23" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D23" s="3" t="s">
@@ -934,13 +940,13 @@
       </c>
     </row>
     <row r="25" spans="4:12" x14ac:dyDescent="0.3">
-      <c r="D25" s="15" t="s">
+      <c r="D25" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="E25" s="15"/>
-      <c r="F25" s="15"/>
-      <c r="G25" s="15"/>
-      <c r="H25" s="15"/>
+      <c r="E25" s="17"/>
+      <c r="F25" s="17"/>
+      <c r="G25" s="17"/>
+      <c r="H25" s="17"/>
     </row>
     <row r="26" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D26" s="3" t="s">
@@ -992,12 +998,12 @@
       <c r="L29" s="1"/>
     </row>
     <row r="31" spans="4:12" x14ac:dyDescent="0.3">
-      <c r="D31" s="16" t="s">
+      <c r="D31" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="E31" s="16"/>
-      <c r="F31" s="16"/>
-      <c r="G31" s="16"/>
+      <c r="E31" s="18"/>
+      <c r="F31" s="18"/>
+      <c r="G31" s="18"/>
     </row>
     <row r="32" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D32" s="4" t="s">
@@ -1010,14 +1016,14 @@
         <v>48</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>27</v>
+        <v>64</v>
       </c>
     </row>
     <row r="34" spans="4:12" x14ac:dyDescent="0.3">
-      <c r="D34" s="16" t="s">
+      <c r="D34" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="E34" s="16"/>
+      <c r="E34" s="18"/>
     </row>
     <row r="35" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D35" s="4" t="s">
@@ -1028,10 +1034,10 @@
       </c>
     </row>
     <row r="37" spans="4:12" x14ac:dyDescent="0.3">
-      <c r="D37" s="16" t="s">
+      <c r="D37" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="E37" s="16"/>
+      <c r="E37" s="18"/>
     </row>
     <row r="38" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D38" s="4" t="s">
@@ -1042,17 +1048,17 @@
       </c>
     </row>
     <row r="40" spans="4:12" x14ac:dyDescent="0.3">
-      <c r="D40" s="11" t="s">
+      <c r="D40" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="E40" s="12"/>
-      <c r="F40" s="12"/>
-      <c r="G40" s="12"/>
-      <c r="H40" s="12"/>
-      <c r="I40" s="12"/>
-      <c r="J40" s="12"/>
-      <c r="K40" s="12"/>
-      <c r="L40" s="13"/>
+      <c r="E40" s="14"/>
+      <c r="F40" s="14"/>
+      <c r="G40" s="14"/>
+      <c r="H40" s="14"/>
+      <c r="I40" s="14"/>
+      <c r="J40" s="14"/>
+      <c r="K40" s="14"/>
+      <c r="L40" s="15"/>
     </row>
     <row r="41" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D41" s="4" t="s">
@@ -1082,12 +1088,12 @@
       <c r="L41" s="5"/>
     </row>
     <row r="43" spans="4:12" x14ac:dyDescent="0.3">
-      <c r="D43" s="11" t="s">
+      <c r="D43" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="E43" s="12"/>
-      <c r="F43" s="12"/>
-      <c r="G43" s="13"/>
+      <c r="E43" s="14"/>
+      <c r="F43" s="14"/>
+      <c r="G43" s="15"/>
     </row>
     <row r="44" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D44" s="4" t="s">
@@ -1097,19 +1103,19 @@
         <v>33</v>
       </c>
       <c r="F44" s="4" t="s">
-        <v>34</v>
+        <v>63</v>
       </c>
       <c r="G44" s="4" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="46" spans="4:12" x14ac:dyDescent="0.3">
-      <c r="D46" s="14" t="s">
+      <c r="D46" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="E46" s="14"/>
-      <c r="F46" s="14"/>
-      <c r="G46" s="14"/>
+      <c r="E46" s="16"/>
+      <c r="F46" s="16"/>
+      <c r="G46" s="16"/>
     </row>
     <row r="47" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D47" s="6" t="s">
@@ -1129,11 +1135,11 @@
       </c>
     </row>
     <row r="49" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D49" s="14" t="s">
+      <c r="D49" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="E49" s="14"/>
-      <c r="F49" s="14"/>
+      <c r="E49" s="16"/>
+      <c r="F49" s="16"/>
     </row>
     <row r="50" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D50" s="6" t="s">
@@ -1150,11 +1156,11 @@
       </c>
     </row>
     <row r="52" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D52" s="14" t="s">
+      <c r="D52" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="E52" s="14"/>
-      <c r="F52" s="14"/>
+      <c r="E52" s="16"/>
+      <c r="F52" s="16"/>
     </row>
     <row r="53" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D53" s="6" t="s">
@@ -1213,11 +1219,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="D4:J4"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="D10:F10"/>
-    <mergeCell ref="D16:G16"/>
-    <mergeCell ref="D13:L13"/>
     <mergeCell ref="D58:I58"/>
     <mergeCell ref="D40:L40"/>
     <mergeCell ref="D52:F52"/>
@@ -1232,6 +1233,11 @@
     <mergeCell ref="D25:H25"/>
     <mergeCell ref="D28:H28"/>
     <mergeCell ref="D31:G31"/>
+    <mergeCell ref="D4:J4"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="D16:G16"/>
+    <mergeCell ref="D13:L13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>